<commit_message>
Final Docs Updated - test cases added
</commit_message>
<xml_diff>
--- a/Assets/#documentation/Testing docs/TEST cases.xlsx
+++ b/Assets/#documentation/Testing docs/TEST cases.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\infinity-services\Assets\#documentation\Testing docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="Build 1.0" sheetId="1" r:id="rId1"/>
+    <sheet name="LOGIN TCs" sheetId="1" r:id="rId1"/>
+    <sheet name="USERS TCs" sheetId="2" r:id="rId2"/>
+    <sheet name=" SPs TCs" sheetId="4" r:id="rId3"/>
+    <sheet name="Admin TCs" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="118">
   <si>
     <t>PROJECT NAME :</t>
   </si>
@@ -64,9 +72,6 @@
     <t>TC-01</t>
   </si>
   <si>
-    <t>Verify login of user</t>
-  </si>
-  <si>
     <t>enter valid user id and password</t>
   </si>
   <si>
@@ -112,140 +117,272 @@
     <t>TC-04</t>
   </si>
   <si>
-    <t>try to access sp from user</t>
-  </si>
-  <si>
-    <t>enter sp URL from user login</t>
-  </si>
-  <si>
-    <t>validate s_type &amp; redirect</t>
-  </si>
-  <si>
-    <t>preempt from access &amp; go to profile</t>
-  </si>
-  <si>
-    <t>redirected to user profile</t>
-  </si>
-  <si>
     <t>TC-05</t>
   </si>
   <si>
-    <t>try to access user from</t>
-  </si>
-  <si>
-    <t>enter user URL from sp login</t>
-  </si>
-  <si>
-    <t>preempt from access &amp; go to bookings</t>
-  </si>
-  <si>
     <t>TC-06</t>
   </si>
   <si>
-    <t>ALL MODULES AS SYSTEM</t>
-  </si>
-  <si>
     <t>book a service</t>
   </si>
   <si>
-    <t>search sp &amp; book service</t>
-  </si>
-  <si>
-    <t>message of success booking</t>
-  </si>
-  <si>
-    <t>enter booking date</t>
-  </si>
-  <si>
-    <t>service booked</t>
-  </si>
-  <si>
     <t>TC-07</t>
   </si>
   <si>
-    <t>accept request from user</t>
-  </si>
-  <si>
-    <t>from bookings accept serv req</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>updated status of service as accepted</t>
-  </si>
-  <si>
-    <t>service accepted</t>
-  </si>
-  <si>
     <t>TC-08</t>
   </si>
   <si>
-    <t>reject request from user</t>
-  </si>
-  <si>
-    <t>from bookings rejectt serv req</t>
-  </si>
-  <si>
-    <t>redirect to change time &amp; status to rejected</t>
-  </si>
-  <si>
-    <t>service rejected</t>
-  </si>
-  <si>
-    <t>TC-09</t>
-  </si>
-  <si>
-    <t>accept change time from sp</t>
-  </si>
-  <si>
-    <t>from bookings accept change time</t>
-  </si>
-  <si>
-    <t>update service status to accepted</t>
-  </si>
-  <si>
-    <t>TC-10</t>
-  </si>
-  <si>
-    <t>completion service update</t>
-  </si>
-  <si>
-    <t>update status of service to complete</t>
-  </si>
-  <si>
-    <t>select completed status op</t>
-  </si>
-  <si>
-    <t>update service status to completed</t>
-  </si>
-  <si>
-    <t>service completed</t>
-  </si>
-  <si>
-    <t>TC-11</t>
-  </si>
-  <si>
-    <t>payment made successfully</t>
-  </si>
-  <si>
-    <t>update pay_status to paid</t>
-  </si>
-  <si>
-    <t>select paid option from list</t>
-  </si>
-  <si>
-    <t>update service pay status to paid</t>
-  </si>
-  <si>
-    <t>service paid</t>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t>LOGIN &amp; REGISTER</t>
+  </si>
+  <si>
+    <t>Verify valid login of user</t>
+  </si>
+  <si>
+    <t>alert for invalid credentials</t>
+  </si>
+  <si>
+    <t>alert of invalid inputs</t>
+  </si>
+  <si>
+    <t>Invalid user id &amp; password</t>
+  </si>
+  <si>
+    <t>Verify invalid login of user</t>
+  </si>
+  <si>
+    <t>Verify invalid login of SP</t>
+  </si>
+  <si>
+    <t>Verify invalid login of Admin</t>
+  </si>
+  <si>
+    <t>verify already registered user</t>
+  </si>
+  <si>
+    <t>verify already registered sp</t>
+  </si>
+  <si>
+    <t>validate already registered user</t>
+  </si>
+  <si>
+    <t>validate already registered sp</t>
+  </si>
+  <si>
+    <t>registered user credentials</t>
+  </si>
+  <si>
+    <t>registered sp credentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alert for already registered </t>
+  </si>
+  <si>
+    <t>USER Module</t>
+  </si>
+  <si>
+    <t>Search for Service providers</t>
+  </si>
+  <si>
+    <t>access dasshboard &amp; search for sp</t>
+  </si>
+  <si>
+    <t>list of available services</t>
+  </si>
+  <si>
+    <t>available services in dashboard</t>
+  </si>
+  <si>
+    <t>click book a service option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">redirect to booking date time </t>
+  </si>
+  <si>
+    <t>redirected to booking date time</t>
+  </si>
+  <si>
+    <t>apply bookings date time</t>
+  </si>
+  <si>
+    <t>enter date and time as wish</t>
+  </si>
+  <si>
+    <t>booking credentials</t>
+  </si>
+  <si>
+    <t>success redirect to bookings</t>
+  </si>
+  <si>
+    <t>redirected to bookings</t>
+  </si>
+  <si>
+    <t>accept changed time</t>
+  </si>
+  <si>
+    <t>select appropriate option of accept</t>
+  </si>
+  <si>
+    <t>accept status</t>
+  </si>
+  <si>
+    <t>update serv_Status to Accepted</t>
+  </si>
+  <si>
+    <t>serv_status updated</t>
+  </si>
+  <si>
+    <t>validate complete status</t>
+  </si>
+  <si>
+    <t>select appropriate option of done</t>
+  </si>
+  <si>
+    <t>completion status</t>
+  </si>
+  <si>
+    <t>update serv_status to completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rate the services </t>
+  </si>
+  <si>
+    <t xml:space="preserve">enter the ratings for service </t>
+  </si>
+  <si>
+    <t>rating stars</t>
+  </si>
+  <si>
+    <t>notify sp about ratings</t>
+  </si>
+  <si>
+    <t>notfied sp for ratings</t>
+  </si>
+  <si>
+    <t>ADMIN Module</t>
+  </si>
+  <si>
+    <t>accept the service request</t>
+  </si>
+  <si>
+    <t>accept request from bookings</t>
+  </si>
+  <si>
+    <t>update status to accepted</t>
+  </si>
+  <si>
+    <t>reject service request</t>
+  </si>
+  <si>
+    <t>reject request &amp; go to change time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">redirect to changed time </t>
+  </si>
+  <si>
+    <t>redirected to change time</t>
+  </si>
+  <si>
+    <t>validate changed time</t>
+  </si>
+  <si>
+    <t>enter time as per comfort</t>
+  </si>
+  <si>
+    <t>changed time</t>
+  </si>
+  <si>
+    <t>update serv_status to changedTime</t>
+  </si>
+  <si>
+    <t>update payment status</t>
+  </si>
+  <si>
+    <t>select appropriate option of payment</t>
+  </si>
+  <si>
+    <t>update serv_status to paid</t>
+  </si>
+  <si>
+    <t>get notify of ratings</t>
+  </si>
+  <si>
+    <t>get notify update after user rate it</t>
+  </si>
+  <si>
+    <t>SERVICE PROVIDER Module</t>
+  </si>
+  <si>
+    <t>after login redirect to dashboard</t>
+  </si>
+  <si>
+    <t>login and redirect to dashboard</t>
+  </si>
+  <si>
+    <t>redirect to admin dashboard</t>
+  </si>
+  <si>
+    <t>redirected to dashboard</t>
+  </si>
+  <si>
+    <t>validate total orders</t>
+  </si>
+  <si>
+    <t>list out total order as table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">table of total order placed </t>
+  </si>
+  <si>
+    <t>table of orders shown</t>
+  </si>
+  <si>
+    <t>validate total users</t>
+  </si>
+  <si>
+    <t>list out total users as table</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">table of total users registered </t>
+  </si>
+  <si>
+    <t>table of total  users shown</t>
+  </si>
+  <si>
+    <t>validate total service providers</t>
+  </si>
+  <si>
+    <t>list out total service Providers table</t>
+  </si>
+  <si>
+    <t>table service providers shown</t>
+  </si>
+  <si>
+    <t>download respective file</t>
+  </si>
+  <si>
+    <t>go to particular page and click download</t>
+  </si>
+  <si>
+    <t>generate &amp; download csv file</t>
+  </si>
+  <si>
+    <t>file downloaded successfully</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -560,7 +697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -568,6 +705,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -586,36 +735,33 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -628,13 +774,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -643,6 +789,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -689,7 +843,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -721,9 +875,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -755,6 +910,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -930,93 +1086,96 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:H17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
     <col min="4" max="4" width="34.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
     <col min="6" max="6" width="37.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="23" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="14"/>
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="2:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B2" s="14" t="s">
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="2:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B3" s="14" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="23" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="2:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B4" s="14" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="23" t="s">
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="2:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B5" s="20" t="s">
+      <c r="F4" s="14"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23" t="s">
+      <c r="C5" s="24"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="2:8" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B6" s="10" t="s">
+      <c r="F5" s="14"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1032,277 +1191,956 @@
         <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="30" customHeight="1">
-      <c r="B7" s="15" t="s">
+    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="15" t="s">
+      <c r="F7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="G7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" ht="30" customHeight="1">
-      <c r="B8" s="15" t="s">
+      <c r="C8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="D9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="G9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="30" customHeight="1">
-      <c r="B9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="15" t="s">
+      <c r="F11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="15" t="s">
+      <c r="G11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="30" customHeight="1">
-      <c r="B10" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="15" t="s">
+      <c r="H11" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="15" t="s">
+      <c r="C12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="15" t="s">
+      <c r="C13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="30" customHeight="1">
-      <c r="B11" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" ht="30" customHeight="1">
-      <c r="B12" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="15" t="s">
+      <c r="C14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="30" customHeight="1">
-      <c r="B13" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="15" t="s">
+      <c r="D14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="15" t="s">
+      <c r="E14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="30" customHeight="1">
-      <c r="B14" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="30" customHeight="1">
-      <c r="B15" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="30" customHeight="1">
-      <c r="B16" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="30" customHeight="1" thickBot="1">
-      <c r="B17" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>22</v>
+      <c r="G14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
     <mergeCell ref="G1:H5"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="14"/>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H5"/>
     <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
     <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
     <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B5:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="14"/>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H5"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B5:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="39.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="33" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="14"/>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H5"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="B5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>